<commit_message>
'Day-6', Completion of 2d array, as now start strings section...
</commit_message>
<xml_diff>
--- a/450 DSA Cracked Questions By Love Babber.xlsx
+++ b/450 DSA Cracked Questions By Love Babber.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DSA C++\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F7BA6C3-7782-428E-A96D-0FF7AF755A51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3169FB4-ED54-4950-9872-562DA01B60EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1786" uniqueCount="472">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1786" uniqueCount="473">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1441,13 +1441,16 @@
   </si>
   <si>
     <t xml:space="preserve">Yes </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Need to do again after DP</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1509,6 +1512,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1531,7 +1542,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1555,6 +1566,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1872,8 +1886,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:E481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B43" workbookViewId="0">
-      <selection activeCell="B51" sqref="B51"/>
+    <sheetView tabSelected="1" topLeftCell="B96" workbookViewId="0">
+      <selection activeCell="B62" sqref="B62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -2426,8 +2440,8 @@
       <c r="C44" s="4" t="s">
         <v>464</v>
       </c>
-      <c r="D44" s="4" t="s">
-        <v>470</v>
+      <c r="D44" s="11" t="s">
+        <v>472</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="21">
@@ -2494,7 +2508,7 @@
         <v>47</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>470</v>
+        <v>464</v>
       </c>
       <c r="D49" s="4" t="s">
         <v>470</v>
@@ -2508,7 +2522,7 @@
         <v>48</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>470</v>
+        <v>464</v>
       </c>
       <c r="D50" s="4" t="s">
         <v>470</v>
@@ -2522,7 +2536,7 @@
         <v>49</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>470</v>
+        <v>464</v>
       </c>
       <c r="D51" s="4" t="s">
         <v>470</v>
@@ -2536,7 +2550,7 @@
         <v>50</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>470</v>
+        <v>464</v>
       </c>
       <c r="D52" s="4" t="s">
         <v>470</v>
@@ -2550,7 +2564,7 @@
         <v>51</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>470</v>
+        <v>464</v>
       </c>
       <c r="D53" s="4" t="s">
         <v>470</v>
@@ -2570,7 +2584,7 @@
         <v>53</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>470</v>
+        <v>464</v>
       </c>
       <c r="D56" s="4" t="s">
         <v>470</v>
@@ -2584,7 +2598,7 @@
         <v>54</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>470</v>
+        <v>464</v>
       </c>
       <c r="D57" s="4" t="s">
         <v>470</v>
@@ -2598,7 +2612,7 @@
         <v>55</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>470</v>
+        <v>464</v>
       </c>
       <c r="D58" s="4"/>
     </row>
@@ -2606,11 +2620,11 @@
       <c r="A59" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="B59" s="7" t="s">
+      <c r="B59" s="6" t="s">
         <v>56</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>470</v>
+        <v>464</v>
       </c>
       <c r="D59" s="4" t="s">
         <v>470</v>
@@ -2624,7 +2638,7 @@
         <v>57</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>470</v>
+        <v>464</v>
       </c>
       <c r="D60" s="4" t="s">
         <v>470</v>
@@ -2638,7 +2652,7 @@
         <v>467</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>470</v>
+        <v>464</v>
       </c>
       <c r="D61" s="4" t="s">
         <v>470</v>
@@ -8740,8 +8754,9 @@
     <hyperlink ref="B2" r:id="rId446" xr:uid="{E07D4FE5-46C7-AC4D-9E01-2300AA43B58A}"/>
     <hyperlink ref="E20" r:id="rId447" xr:uid="{2A0057E0-EBE3-4B58-BDFA-E403F929D9DF}"/>
     <hyperlink ref="E61" r:id="rId448" xr:uid="{7F8C7863-377E-4C33-801A-3A53FE61D1F3}"/>
+    <hyperlink ref="B59" r:id="rId449" xr:uid="{D3B339F1-7390-4FE7-9E63-C6F5A1376975}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId449"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId450"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
'Day-7', Doing recursion in strings
</commit_message>
<xml_diff>
--- a/450 DSA Cracked Questions By Love Babber.xlsx
+++ b/450 DSA Cracked Questions By Love Babber.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DSA C++\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3169FB4-ED54-4950-9872-562DA01B60EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B98063A1-E625-43AC-8F83-49047A78CA75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1786" uniqueCount="473">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1785" uniqueCount="473">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1887,7 +1887,7 @@
   <dimension ref="A1:E481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B96" workbookViewId="0">
-      <selection activeCell="B62" sqref="B62"/>
+      <selection activeCell="B97" sqref="B97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -3171,11 +3171,9 @@
         <v>94</v>
       </c>
       <c r="C98" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D98" s="4" t="s">
-        <v>3</v>
-      </c>
+        <v>464</v>
+      </c>
+      <c r="D98" s="4"/>
     </row>
     <row r="100" spans="1:4" ht="21">
       <c r="A100" s="8"/>

</xml_diff>